<commit_message>
Add DataType and Console Class Example
</commit_message>
<xml_diff>
--- a/C#_Topics.xlsx
+++ b/C#_Topics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="6780"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>S.No</t>
   </si>
@@ -44,13 +44,16 @@
     <t>Chapter-2 C#.NET Basics</t>
   </si>
   <si>
+    <t>On Progress</t>
+  </si>
+  <si>
     <t>Chapter-3 OOPs in C#</t>
   </si>
   <si>
     <t>Chapter-4 Exception Handling</t>
   </si>
   <si>
-    <t>On Progress</t>
+    <t>Finshed</t>
   </si>
   <si>
     <t>Chapter-5 Events, Delegates, and Lambda Expression in C#</t>
@@ -60,9 +63,6 @@
   </si>
   <si>
     <t>Chapter-7 Collections in C#</t>
-  </si>
-  <si>
-    <t>Finshed</t>
   </si>
   <si>
     <t>Chapter-8 File Handling</t>
@@ -267,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,12 +354,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -445,12 +439,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,68 +671,68 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -771,9 +759,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1311,7 +1296,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1341,32 +1326,34 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1374,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1383,7 +1370,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -1392,10 +1379,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1405,8 +1392,8 @@
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">

</xml_diff>